<commit_message>
Data ready for upload to SQL database
</commit_message>
<xml_diff>
--- a/Data/cost_quality/Qual_Grower_Trend_Country.xlsx
+++ b/Data/cost_quality/Qual_Grower_Trend_Country.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Desktop\Projects\UT-DataBC-Project-2\Data\cost_quality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4250CA2E-E5A6-4194-AE22-166C326BCC12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD3C89F-2039-4EDC-AD41-0AA69B36E43E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$66</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -358,7 +369,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,17 +405,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -676,12 +703,19 @@
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="17" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="18.85546875" style="4" customWidth="1"/>
+    <col min="6" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="7.28515625" style="1" customWidth="1"/>
+    <col min="15" max="17" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -697,7 +731,7 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>97</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -736,387 +770,387 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.53009089236090667</v>
+        <v>9</v>
+      </c>
+      <c r="E2" s="4">
+        <v>23.2225</v>
       </c>
       <c r="F2" s="1">
-        <v>7.5485714285714289</v>
+        <v>7.833333333333333</v>
       </c>
       <c r="G2" s="1">
-        <v>7.5545833333333343</v>
+        <v>7.7766666666666664</v>
       </c>
       <c r="H2" s="1">
-        <v>7.3641666666666659</v>
+        <v>7.6099999999999994</v>
       </c>
       <c r="I2" s="1">
-        <v>7.4754166666666668</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="J2" s="1">
-        <v>7.5379166666666668</v>
+        <v>7.78</v>
       </c>
       <c r="K2" s="1">
-        <v>7.5870833333333332</v>
+        <v>7.75</v>
       </c>
       <c r="L2" s="1">
-        <v>9.9720833333333339</v>
+        <v>10</v>
       </c>
       <c r="M2" s="1">
-        <v>9.8612500000000001</v>
+        <v>10</v>
       </c>
       <c r="N2" s="1">
-        <v>10</v>
+        <v>9.7766666666666655</v>
       </c>
       <c r="O2" s="1">
-        <v>7.5691666666666686</v>
+        <v>7.6400000000000006</v>
       </c>
       <c r="P2" s="1">
-        <v>82.470238095238102</v>
+        <v>83.5</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.49180232517977074</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="4">
+        <v>22.62166666666667</v>
       </c>
       <c r="F3" s="1">
-        <v>7.6475000000000009</v>
+        <v>7.625</v>
       </c>
       <c r="G3" s="1">
-        <v>7.5670000000000002</v>
+        <v>7.625</v>
       </c>
       <c r="H3" s="1">
-        <v>7.4510000000000005</v>
+        <v>7.415</v>
       </c>
       <c r="I3" s="1">
-        <v>7.5250000000000004</v>
+        <v>7.585</v>
       </c>
       <c r="J3" s="1">
-        <v>7.660000000000001</v>
+        <v>7.665</v>
       </c>
       <c r="K3" s="1">
-        <v>7.6669999999999998</v>
+        <v>8.0449999999999999</v>
       </c>
       <c r="L3" s="1">
-        <v>9.9329999999999998</v>
+        <v>9.6649999999999991</v>
       </c>
       <c r="M3" s="1">
-        <v>9.9329999999999998</v>
+        <v>9.6649999999999991</v>
       </c>
       <c r="N3" s="1">
-        <v>10</v>
+        <v>9.33</v>
       </c>
       <c r="O3" s="1">
-        <v>7.6340000000000003</v>
+        <v>7.4550000000000001</v>
       </c>
       <c r="P3" s="1">
-        <v>83.017499999999998</v>
+        <v>82.074999999999989</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="1">
-        <v>0.47582339330249557</v>
+      <c r="E4" s="4">
+        <v>21.2425</v>
       </c>
       <c r="F4" s="1">
-        <v>8.2949999999999999</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>7.92</v>
+        <v>7.8033333333333337</v>
       </c>
       <c r="H4" s="1">
-        <v>7.96</v>
+        <v>7.9733333333333336</v>
       </c>
       <c r="I4" s="1">
-        <v>7.75</v>
+        <v>8.0533333333333328</v>
       </c>
       <c r="J4" s="1">
-        <v>8.125</v>
+        <v>7.3633333333333333</v>
       </c>
       <c r="K4" s="1">
-        <v>8</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="L4" s="1">
         <v>10</v>
       </c>
       <c r="M4" s="1">
-        <v>10</v>
+        <v>9.7766666666666655</v>
       </c>
       <c r="N4" s="1">
-        <v>10</v>
+        <v>9.7766666666666655</v>
       </c>
       <c r="O4" s="1">
-        <v>8.125</v>
+        <v>7.5266666666666664</v>
       </c>
       <c r="P4" s="1">
-        <v>86.174999999999997</v>
+        <v>75.94</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.4590610948309054</v>
+        <v>5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>18.420000000000002</v>
       </c>
       <c r="F5" s="1">
-        <v>7.4627777777777773</v>
+        <v>7.8900000000000006</v>
       </c>
       <c r="G5" s="1">
-        <v>7.4485714285714284</v>
+        <v>7.8066666666666675</v>
       </c>
       <c r="H5" s="1">
-        <v>7.4090476190476195</v>
+        <v>7.5266666666666664</v>
       </c>
       <c r="I5" s="1">
-        <v>7.4804761904761907</v>
+        <v>7.3900000000000006</v>
       </c>
       <c r="J5" s="1">
-        <v>7.4719047619047627</v>
+        <v>7.5533333333333337</v>
       </c>
       <c r="K5" s="1">
-        <v>7.3971428571428559</v>
+        <v>7.7233333333333336</v>
       </c>
       <c r="L5" s="1">
-        <v>9.8409523809523822</v>
+        <v>9.7766666666666655</v>
       </c>
       <c r="M5" s="1">
-        <v>9.9047619047619051</v>
+        <v>10</v>
       </c>
       <c r="N5" s="1">
-        <v>9.9680952380952395</v>
+        <v>10</v>
       </c>
       <c r="O5" s="1">
-        <v>7.5433333333333321</v>
+        <v>7.7233333333333336</v>
       </c>
       <c r="P5" s="1">
-        <v>81.927063492063496</v>
+        <v>83.39</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.4482642603784403</v>
+        <v>17</v>
+      </c>
+      <c r="E6" s="4">
+        <v>17.309999999999999</v>
       </c>
       <c r="F6" s="1">
-        <v>7.4514285714285711</v>
+        <v>7.5266666666666673</v>
       </c>
       <c r="G6" s="1">
-        <v>7.4994999999999994</v>
+        <v>7.541666666666667</v>
       </c>
       <c r="H6" s="1">
-        <v>7.4134999999999991</v>
+        <v>7.4866666666666672</v>
       </c>
       <c r="I6" s="1">
-        <v>7.4000000000000012</v>
+        <v>7.5966666666666667</v>
       </c>
       <c r="J6" s="1">
-        <v>7.479000000000001</v>
+        <v>7.6233333333333322</v>
       </c>
       <c r="K6" s="1">
-        <v>7.4740000000000011</v>
+        <v>7.5866666666666669</v>
       </c>
       <c r="L6" s="1">
-        <v>9.9664999999999999</v>
+        <v>10</v>
       </c>
       <c r="M6" s="1">
-        <v>9.7999999999999989</v>
+        <v>10</v>
       </c>
       <c r="N6" s="1">
-        <v>9.7664999999999988</v>
+        <v>9.8883333333333336</v>
       </c>
       <c r="O6" s="1">
-        <v>7.4704999999999995</v>
+        <v>7.4849999999999994</v>
       </c>
       <c r="P6" s="1">
-        <v>81.720928571428573</v>
+        <v>82.735000000000014</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="1">
-        <v>0.4366026950914762</v>
+      <c r="E7" s="4">
+        <v>16.9375</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>7.53</v>
       </c>
       <c r="G7" s="1">
-        <v>7.4553333333333329</v>
+        <v>7.416666666666667</v>
       </c>
       <c r="H7" s="1">
-        <v>7.3493333333333339</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="I7" s="1">
-        <v>7.4993333333333334</v>
+        <v>7.413333333333334</v>
       </c>
       <c r="J7" s="1">
-        <v>7.5</v>
+        <v>7.583333333333333</v>
       </c>
       <c r="K7" s="1">
-        <v>7.3386666666666667</v>
+        <v>7.6933333333333325</v>
       </c>
       <c r="L7" s="1">
-        <v>9.4666666666666668</v>
+        <v>10</v>
       </c>
       <c r="M7" s="1">
-        <v>9.4666666666666668</v>
+        <v>10</v>
       </c>
       <c r="N7" s="1">
-        <v>10</v>
+        <v>9.7766666666666655</v>
       </c>
       <c r="O7" s="1">
-        <v>7.4613333333333332</v>
+        <v>7.4733333333333336</v>
       </c>
       <c r="P7" s="1">
-        <v>73.537333333333322</v>
+        <v>82.22</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.36837686207401454</v>
+        <v>13</v>
+      </c>
+      <c r="E8" s="4">
+        <v>15.31</v>
       </c>
       <c r="F8" s="1">
-        <v>7.6249999999999982</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>7.6</v>
+        <v>7.83</v>
       </c>
       <c r="H8" s="1">
-        <v>7.4084999999999992</v>
+        <v>7.83</v>
       </c>
       <c r="I8" s="1">
-        <v>7.5004999999999979</v>
+        <v>8.08</v>
       </c>
       <c r="J8" s="1">
-        <v>7.508</v>
+        <v>7.83</v>
       </c>
       <c r="K8" s="1">
-        <v>7.5129999999999999</v>
+        <v>7.83</v>
       </c>
       <c r="L8" s="1">
-        <v>9.9664999999999999</v>
+        <v>10</v>
       </c>
       <c r="M8" s="1">
-        <v>9.9664999999999999</v>
+        <v>10</v>
       </c>
       <c r="N8" s="1">
-        <v>9.9664999999999999</v>
+        <v>10</v>
       </c>
       <c r="O8" s="1">
-        <v>7.4970000000000017</v>
+        <v>7.92</v>
       </c>
       <c r="P8" s="1">
-        <v>82.55149999999999</v>
+        <v>77.320000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="1">
-        <v>0.31650251535769169</v>
+      <c r="E9" s="4">
+        <v>4.6919979251810737</v>
       </c>
       <c r="F9" s="1">
-        <v>8.017142857142856</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1">
-        <v>7.9226666666666672</v>
+        <v>6.5</v>
       </c>
       <c r="H9" s="1">
-        <v>7.6773333333333333</v>
+        <v>6.5</v>
       </c>
       <c r="I9" s="1">
-        <v>7.722666666666667</v>
+        <v>7.17</v>
       </c>
       <c r="J9" s="1">
-        <v>7.6779999999999999</v>
+        <v>7</v>
       </c>
       <c r="K9" s="1">
-        <v>7.7273333333333332</v>
+        <v>6.83</v>
       </c>
       <c r="L9" s="1">
         <v>10</v>
@@ -1128,10 +1162,10 @@
         <v>10</v>
       </c>
       <c r="O9" s="1">
-        <v>7.7393333333333336</v>
+        <v>6.17</v>
       </c>
       <c r="P9" s="1">
-        <v>84.484476190476187</v>
+        <v>70.17</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1139,184 +1173,184 @@
         <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.49934343814091448</v>
+        <v>61</v>
+      </c>
+      <c r="E10" s="4">
+        <v>4.221413459416393</v>
       </c>
       <c r="F10" s="1">
-        <v>7.6492500000000021</v>
+        <v>7.4574999999999996</v>
       </c>
       <c r="G10" s="1">
-        <v>7.5567499999999983</v>
+        <v>7.5225000000000009</v>
       </c>
       <c r="H10" s="1">
-        <v>7.5187499999999998</v>
+        <v>7.3324999999999996</v>
       </c>
       <c r="I10" s="1">
-        <v>7.5667500000000008</v>
+        <v>7.3949999999999996</v>
       </c>
       <c r="J10" s="1">
-        <v>7.5975000000000037</v>
+        <v>7.4399999999999995</v>
       </c>
       <c r="K10" s="1">
-        <v>7.7082500000000014</v>
+        <v>7.6050000000000004</v>
       </c>
       <c r="L10" s="1">
-        <v>9.9</v>
+        <v>10</v>
       </c>
       <c r="M10" s="1">
-        <v>9.8167500000000008</v>
+        <v>10</v>
       </c>
       <c r="N10" s="1">
-        <v>9.9167500000000004</v>
+        <v>10</v>
       </c>
       <c r="O10" s="1">
-        <v>7.625</v>
+        <v>7.3975000000000009</v>
       </c>
       <c r="P10" s="1">
-        <v>82.85575</v>
+        <v>82.15</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.47820653504072869</v>
+        <v>9</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3.9485399566793209</v>
       </c>
       <c r="F11" s="1">
-        <v>7.7953333333333328</v>
+        <v>6.83</v>
       </c>
       <c r="G11" s="1">
-        <v>7.6970000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="H11" s="1">
-        <v>7.6570000000000009</v>
+        <v>6.5</v>
       </c>
       <c r="I11" s="1">
-        <v>7.7080000000000002</v>
+        <v>6.92</v>
       </c>
       <c r="J11" s="1">
-        <v>7.7580000000000009</v>
+        <v>6.75</v>
       </c>
       <c r="K11" s="1">
-        <v>7.7209999999999992</v>
+        <v>7</v>
       </c>
       <c r="L11" s="1">
-        <v>9.833499999999999</v>
+        <v>9.33</v>
       </c>
       <c r="M11" s="1">
         <v>10</v>
       </c>
       <c r="N11" s="1">
-        <v>10</v>
+        <v>9.33</v>
       </c>
       <c r="O11" s="1">
-        <v>7.6709999999999994</v>
+        <v>6.67</v>
       </c>
       <c r="P11" s="1">
-        <v>83.840833333333336</v>
+        <v>75.83</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.45999930313195392</v>
+        <v>9</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3.665191842006764</v>
       </c>
       <c r="F12" s="1">
-        <v>7.6574074074074074</v>
+        <v>7.4843478260869585</v>
       </c>
       <c r="G12" s="1">
-        <v>7.6574074074074074</v>
+        <v>7.3839130434782616</v>
       </c>
       <c r="H12" s="1">
-        <v>7.5637037037037045</v>
+        <v>7.2078260869565254</v>
       </c>
       <c r="I12" s="1">
-        <v>7.5899999999999972</v>
+        <v>7.5452173913043472</v>
       </c>
       <c r="J12" s="1">
-        <v>7.623703703703705</v>
+        <v>7.4528260869565202</v>
       </c>
       <c r="K12" s="1">
-        <v>7.7455555555555575</v>
+        <v>7.463043478260869</v>
       </c>
       <c r="L12" s="1">
-        <v>9.975185185185186</v>
+        <v>9.7391304347826093</v>
       </c>
       <c r="M12" s="1">
-        <v>9.975185185185186</v>
+        <v>9.7099999999999991</v>
       </c>
       <c r="N12" s="1">
-        <v>10</v>
+        <v>9.6663043478260864</v>
       </c>
       <c r="O12" s="1">
-        <v>7.6629629629629621</v>
+        <v>7.3393478260869554</v>
       </c>
       <c r="P12" s="1">
-        <v>83.451111111111103</v>
+        <v>80.991956521739141</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0.45101641684936328</v>
+        <v>61</v>
+      </c>
+      <c r="E13" s="4">
+        <v>3.6278369683268235</v>
       </c>
       <c r="F13" s="1">
-        <v>7.7766666666666664</v>
+        <v>8.017142857142856</v>
       </c>
       <c r="G13" s="1">
-        <v>7.6320000000000006</v>
+        <v>7.9226666666666672</v>
       </c>
       <c r="H13" s="1">
-        <v>7.516</v>
+        <v>7.6773333333333333</v>
       </c>
       <c r="I13" s="1">
-        <v>7.548</v>
+        <v>7.722666666666667</v>
       </c>
       <c r="J13" s="1">
-        <v>7.6820000000000004</v>
+        <v>7.6779999999999999</v>
       </c>
       <c r="K13" s="1">
-        <v>7.831999999999999</v>
+        <v>7.7273333333333332</v>
       </c>
       <c r="L13" s="1">
         <v>10</v>
@@ -1328,198 +1362,198 @@
         <v>10</v>
       </c>
       <c r="O13" s="1">
-        <v>7.65</v>
+        <v>7.7393333333333336</v>
       </c>
       <c r="P13" s="1">
-        <v>83.636666666666684</v>
+        <v>84.484476190476187</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.40994571642614863</v>
+        <v>9</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3.5530419676240541</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>7.73</v>
       </c>
       <c r="G14" s="1">
-        <v>7.42</v>
+        <v>7.6650000000000009</v>
       </c>
       <c r="H14" s="1">
-        <v>7.33</v>
+        <v>7.5625</v>
       </c>
       <c r="I14" s="1">
-        <v>7.33</v>
+        <v>7.8949999999999996</v>
       </c>
       <c r="J14" s="1">
-        <v>7.67</v>
+        <v>7.73</v>
       </c>
       <c r="K14" s="1">
-        <v>7.83</v>
+        <v>7.77</v>
       </c>
       <c r="L14" s="1">
-        <v>10</v>
+        <v>9.8324999999999996</v>
       </c>
       <c r="M14" s="1">
-        <v>10</v>
+        <v>9.8324999999999996</v>
       </c>
       <c r="N14" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O14" s="1">
-        <v>7.58</v>
+        <v>7.6675000000000004</v>
       </c>
       <c r="P14" s="1">
-        <v>75.16</v>
+        <v>82.685000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.35532062345461374</v>
+        <v>5</v>
+      </c>
+      <c r="E15" s="4">
+        <v>3.4195018545660032</v>
       </c>
       <c r="F15" s="1">
-        <v>7.7020833333333343</v>
+        <v>7.2925000000000004</v>
       </c>
       <c r="G15" s="1">
-        <v>7.6246428571428586</v>
+        <v>7.3125</v>
       </c>
       <c r="H15" s="1">
-        <v>7.569642857142858</v>
+        <v>7.1675000000000004</v>
       </c>
       <c r="I15" s="1">
-        <v>7.6692857142857163</v>
+        <v>7.5024999999999995</v>
       </c>
       <c r="J15" s="1">
-        <v>7.6696428571428603</v>
+        <v>7.2900000000000009</v>
       </c>
       <c r="K15" s="1">
-        <v>7.803928571428572</v>
+        <v>7.23</v>
       </c>
       <c r="L15" s="1">
-        <v>9.97607142857143</v>
+        <v>10</v>
       </c>
       <c r="M15" s="1">
         <v>10</v>
       </c>
       <c r="N15" s="1">
-        <v>9.8810714285714294</v>
+        <v>10</v>
       </c>
       <c r="O15" s="1">
-        <v>7.6935714285714294</v>
+        <v>7.2274999999999991</v>
       </c>
       <c r="P15" s="1">
-        <v>83.589940476190492</v>
+        <v>81.022500000000008</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0.34013711562558707</v>
+        <v>11</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3.3752645850487371</v>
       </c>
       <c r="F16" s="1">
-        <v>7.6373333333333315</v>
+        <v>7.5670967741935486</v>
       </c>
       <c r="G16" s="1">
-        <v>7.6216666666666697</v>
+        <v>7.5196774193548359</v>
       </c>
       <c r="H16" s="1">
-        <v>7.576666666666668</v>
+        <v>7.2638709677419353</v>
       </c>
       <c r="I16" s="1">
-        <v>7.5636666666666663</v>
+        <v>7.6183870967741942</v>
       </c>
       <c r="J16" s="1">
-        <v>7.6466666666666674</v>
+        <v>7.4490322580645136</v>
       </c>
       <c r="K16" s="1">
-        <v>7.6473333333333322</v>
+        <v>7.4822580645161256</v>
       </c>
       <c r="L16" s="1">
-        <v>9.9333333333333353</v>
+        <v>9.8706451612903212</v>
       </c>
       <c r="M16" s="1">
-        <v>9.9556666666666676</v>
+        <v>9.9351612903225792</v>
       </c>
       <c r="N16" s="1">
-        <v>9.9556666666666676</v>
+        <v>9.9567741935483856</v>
       </c>
       <c r="O16" s="1">
-        <v>7.6140000000000008</v>
+        <v>7.4009677419354833</v>
       </c>
       <c r="P16" s="1">
-        <v>83.152000000000015</v>
+        <v>82.06387096774192</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0.23688748084350145</v>
+        <v>19</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3.222246160840029</v>
       </c>
       <c r="F17" s="1">
-        <v>7.4574999999999996</v>
+        <v>7.7572727272727269</v>
       </c>
       <c r="G17" s="1">
-        <v>7.5225000000000009</v>
+        <v>7.5283333333333333</v>
       </c>
       <c r="H17" s="1">
-        <v>7.3324999999999996</v>
+        <v>7.5425000000000004</v>
       </c>
       <c r="I17" s="1">
-        <v>7.3949999999999996</v>
+        <v>7.5150000000000006</v>
       </c>
       <c r="J17" s="1">
-        <v>7.4399999999999995</v>
+        <v>7.4016666666666664</v>
       </c>
       <c r="K17" s="1">
-        <v>7.6050000000000004</v>
+        <v>7.6125000000000007</v>
       </c>
       <c r="L17" s="1">
-        <v>10</v>
+        <v>9.7225000000000001</v>
       </c>
       <c r="M17" s="1">
         <v>10</v>
@@ -1528,95 +1562,95 @@
         <v>10</v>
       </c>
       <c r="O17" s="1">
-        <v>7.3975000000000009</v>
+        <v>7.6883333333333335</v>
       </c>
       <c r="P17" s="1">
-        <v>82.15</v>
+        <v>82.768106060606058</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0.36309840748134359</v>
+        <v>9</v>
+      </c>
+      <c r="E18" s="4">
+        <v>3.1099831139399892</v>
       </c>
       <c r="F18" s="1">
-        <v>7.6037499999999998</v>
+        <v>7.335</v>
       </c>
       <c r="G18" s="1">
-        <v>7.4175000000000004</v>
+        <v>7.5</v>
       </c>
       <c r="H18" s="1">
-        <v>7.4587500000000002</v>
+        <v>7.375</v>
       </c>
       <c r="I18" s="1">
-        <v>7.52</v>
+        <v>7.375</v>
       </c>
       <c r="J18" s="1">
-        <v>7.5625</v>
+        <v>7.54</v>
       </c>
       <c r="K18" s="1">
-        <v>7.51</v>
+        <v>7.5</v>
       </c>
       <c r="L18" s="1">
-        <v>9.75</v>
+        <v>10</v>
       </c>
       <c r="M18" s="1">
-        <v>9.75</v>
+        <v>10</v>
       </c>
       <c r="N18" s="1">
         <v>10</v>
       </c>
       <c r="O18" s="1">
-        <v>7.7074999999999996</v>
+        <v>7.5449999999999999</v>
       </c>
       <c r="P18" s="1">
-        <v>82.279999999999987</v>
+        <v>82.17</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0.35042625609375322</v>
+        <v>19</v>
+      </c>
+      <c r="E19" s="4">
+        <v>3.07584180675823</v>
       </c>
       <c r="F19" s="1">
-        <v>7.605714285714285</v>
+        <v>7.6219999999999999</v>
       </c>
       <c r="G19" s="1">
-        <v>7.63</v>
+        <v>7.5837500000000002</v>
       </c>
       <c r="H19" s="1">
-        <v>7.6071428571428568</v>
+        <v>7.2543749999999996</v>
       </c>
       <c r="I19" s="1">
-        <v>7.7157142857142853</v>
+        <v>7.6725000000000003</v>
       </c>
       <c r="J19" s="1">
-        <v>7.6214285714285719</v>
+        <v>7.5006250000000003</v>
       </c>
       <c r="K19" s="1">
-        <v>7.62</v>
+        <v>7.4125000000000005</v>
       </c>
       <c r="L19" s="1">
         <v>10</v>
@@ -1628,10 +1662,10 @@
         <v>10</v>
       </c>
       <c r="O19" s="1">
-        <v>7.75</v>
+        <v>7.375</v>
       </c>
       <c r="P19" s="1">
-        <v>83.55</v>
+        <v>82.420749999999998</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1639,284 +1673,284 @@
         <v>70</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0.34632890562408336</v>
+        <v>43</v>
+      </c>
+      <c r="E20" s="4">
+        <v>3.0486873863219222</v>
       </c>
       <c r="F20" s="1">
-        <v>7.6668750000000001</v>
+        <v>7.58</v>
       </c>
       <c r="G20" s="1">
-        <v>7.5243749999999991</v>
+        <v>7.71</v>
       </c>
       <c r="H20" s="1">
-        <v>7.4993749999999997</v>
+        <v>7.7949999999999999</v>
       </c>
       <c r="I20" s="1">
-        <v>7.5006249999999994</v>
+        <v>7.75</v>
       </c>
       <c r="J20" s="1">
-        <v>7.5093749999999995</v>
+        <v>7.75</v>
       </c>
       <c r="K20" s="1">
-        <v>7.6918749999999996</v>
+        <v>7.665</v>
       </c>
       <c r="L20" s="1">
-        <v>9.9168749999999992</v>
+        <v>10</v>
       </c>
       <c r="M20" s="1">
-        <v>9.75</v>
+        <v>10</v>
       </c>
       <c r="N20" s="1">
-        <v>9.958124999999999</v>
+        <v>10</v>
       </c>
       <c r="O20" s="1">
-        <v>7.546875</v>
+        <v>7.835</v>
       </c>
       <c r="P20" s="1">
-        <v>82.564374999999984</v>
+        <v>84.084999999999994</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0.32801001653582013</v>
+        <v>17</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2.9927879337159</v>
       </c>
       <c r="F21" s="1">
-        <v>7.58</v>
+        <v>7.6385000000000005</v>
       </c>
       <c r="G21" s="1">
-        <v>7.71</v>
+        <v>7.6289999999999996</v>
       </c>
       <c r="H21" s="1">
-        <v>7.7949999999999999</v>
+        <v>7.4164999999999992</v>
       </c>
       <c r="I21" s="1">
-        <v>7.75</v>
+        <v>7.7410000000000014</v>
       </c>
       <c r="J21" s="1">
-        <v>7.75</v>
+        <v>7.596000000000001</v>
       </c>
       <c r="K21" s="1">
-        <v>7.665</v>
+        <v>7.5205000000000002</v>
       </c>
       <c r="L21" s="1">
-        <v>10</v>
+        <v>9.9330000000000016</v>
       </c>
       <c r="M21" s="1">
-        <v>10</v>
+        <v>9.9330000000000016</v>
       </c>
       <c r="N21" s="1">
-        <v>10</v>
+        <v>9.9330000000000016</v>
       </c>
       <c r="O21" s="1">
-        <v>7.835</v>
+        <v>7.5329999999999995</v>
       </c>
       <c r="P21" s="1">
-        <v>84.084999999999994</v>
+        <v>82.873500000000007</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.31034252198140666</v>
+        <v>43</v>
+      </c>
+      <c r="E22" s="4">
+        <v>2.9635295113658011</v>
       </c>
       <c r="F22" s="1">
-        <v>7.7572727272727269</v>
+        <v>7.5151851851851852</v>
       </c>
       <c r="G22" s="1">
-        <v>7.5283333333333333</v>
+        <v>7.5188888888888874</v>
       </c>
       <c r="H22" s="1">
-        <v>7.5425000000000004</v>
+        <v>7.2774074074074075</v>
       </c>
       <c r="I22" s="1">
-        <v>7.5150000000000006</v>
+        <v>7.549999999999998</v>
       </c>
       <c r="J22" s="1">
-        <v>7.4016666666666664</v>
+        <v>7.4907407407407405</v>
       </c>
       <c r="K22" s="1">
-        <v>7.6125000000000007</v>
+        <v>7.4759259259259245</v>
       </c>
       <c r="L22" s="1">
-        <v>9.7225000000000001</v>
+        <v>9.8022222222222233</v>
       </c>
       <c r="M22" s="1">
-        <v>10</v>
+        <v>9.9011111111111134</v>
       </c>
       <c r="N22" s="1">
-        <v>10</v>
+        <v>9.9011111111111134</v>
       </c>
       <c r="O22" s="1">
-        <v>7.6883333333333335</v>
+        <v>7.4940740740740752</v>
       </c>
       <c r="P22" s="1">
-        <v>82.768106060606058</v>
+        <v>81.926666666666662</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="1">
-        <v>0.28144896939360037</v>
+      <c r="E23" s="4">
+        <v>2.9399908274072941</v>
       </c>
       <c r="F23" s="1">
-        <v>7.73</v>
+        <v>7.6373333333333315</v>
       </c>
       <c r="G23" s="1">
-        <v>7.6650000000000009</v>
+        <v>7.6216666666666697</v>
       </c>
       <c r="H23" s="1">
-        <v>7.5625</v>
+        <v>7.576666666666668</v>
       </c>
       <c r="I23" s="1">
-        <v>7.8949999999999996</v>
+        <v>7.5636666666666663</v>
       </c>
       <c r="J23" s="1">
-        <v>7.73</v>
+        <v>7.6466666666666674</v>
       </c>
       <c r="K23" s="1">
-        <v>7.77</v>
+        <v>7.6473333333333322</v>
       </c>
       <c r="L23" s="1">
-        <v>9.8324999999999996</v>
+        <v>9.9333333333333353</v>
       </c>
       <c r="M23" s="1">
-        <v>9.8324999999999996</v>
+        <v>9.9556666666666676</v>
       </c>
       <c r="N23" s="1">
-        <v>9</v>
+        <v>9.9556666666666676</v>
       </c>
       <c r="O23" s="1">
-        <v>7.6675000000000004</v>
+        <v>7.6140000000000008</v>
       </c>
       <c r="P23" s="1">
-        <v>82.685000000000002</v>
+        <v>83.152000000000015</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0.4811764709912037</v>
+        <v>11</v>
+      </c>
+      <c r="E24" s="4">
+        <v>2.8874286372314319</v>
       </c>
       <c r="F24" s="1">
-        <v>7.5</v>
+        <v>7.6668750000000001</v>
       </c>
       <c r="G24" s="1">
-        <v>7.67</v>
+        <v>7.5243749999999991</v>
       </c>
       <c r="H24" s="1">
-        <v>7.58</v>
+        <v>7.4993749999999997</v>
       </c>
       <c r="I24" s="1">
-        <v>7.75</v>
+        <v>7.5006249999999994</v>
       </c>
       <c r="J24" s="1">
-        <v>7.83</v>
+        <v>7.5093749999999995</v>
       </c>
       <c r="K24" s="1">
-        <v>7.83</v>
+        <v>7.6918749999999996</v>
       </c>
       <c r="L24" s="1">
-        <v>10</v>
+        <v>9.9168749999999992</v>
       </c>
       <c r="M24" s="1">
-        <v>10</v>
+        <v>9.75</v>
       </c>
       <c r="N24" s="1">
-        <v>10</v>
+        <v>9.958124999999999</v>
       </c>
       <c r="O24" s="1">
-        <v>7.67</v>
+        <v>7.546875</v>
       </c>
       <c r="P24" s="1">
-        <v>83.83</v>
+        <v>82.564374999999984</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1">
-        <v>6.531678641410843E-2</v>
+        <v>17</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2.8536674481733448</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <v>7.605714285714285</v>
       </c>
       <c r="G25" s="1">
-        <v>7.83</v>
+        <v>7.63</v>
       </c>
       <c r="H25" s="1">
-        <v>7.83</v>
+        <v>7.6071428571428568</v>
       </c>
       <c r="I25" s="1">
-        <v>8.08</v>
+        <v>7.7157142857142853</v>
       </c>
       <c r="J25" s="1">
-        <v>7.83</v>
+        <v>7.6214285714285719</v>
       </c>
       <c r="K25" s="1">
-        <v>7.83</v>
+        <v>7.62</v>
       </c>
       <c r="L25" s="1">
         <v>10</v>
@@ -1928,118 +1962,118 @@
         <v>10</v>
       </c>
       <c r="O25" s="1">
-        <v>7.92</v>
+        <v>7.75</v>
       </c>
       <c r="P25" s="1">
-        <v>77.320000000000007</v>
+        <v>83.55</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="1">
-        <v>5.9040590405904071E-2</v>
+        <v>11</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2.8143595783365312</v>
       </c>
       <c r="F26" s="1">
-        <v>7.53</v>
+        <v>7.7020833333333343</v>
       </c>
       <c r="G26" s="1">
-        <v>7.416666666666667</v>
+        <v>7.6246428571428586</v>
       </c>
       <c r="H26" s="1">
-        <v>7.333333333333333</v>
+        <v>7.569642857142858</v>
       </c>
       <c r="I26" s="1">
-        <v>7.413333333333334</v>
+        <v>7.6692857142857163</v>
       </c>
       <c r="J26" s="1">
-        <v>7.583333333333333</v>
+        <v>7.6696428571428603</v>
       </c>
       <c r="K26" s="1">
-        <v>7.6933333333333325</v>
+        <v>7.803928571428572</v>
       </c>
       <c r="L26" s="1">
-        <v>10</v>
+        <v>9.97607142857143</v>
       </c>
       <c r="M26" s="1">
         <v>10</v>
       </c>
       <c r="N26" s="1">
-        <v>9.7766666666666655</v>
+        <v>9.8810714285714294</v>
       </c>
       <c r="O26" s="1">
-        <v>7.4733333333333336</v>
+        <v>7.6935714285714294</v>
       </c>
       <c r="P26" s="1">
-        <v>82.22</v>
+        <v>83.589940476190492</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="1">
-        <v>5.777007510109762E-2</v>
+        <v>9</v>
+      </c>
+      <c r="E27" s="4">
+        <v>2.8103211370740082</v>
       </c>
       <c r="F27" s="1">
-        <v>7.5266666666666673</v>
+        <v>7.6249999999999982</v>
       </c>
       <c r="G27" s="1">
-        <v>7.541666666666667</v>
+        <v>7.6</v>
       </c>
       <c r="H27" s="1">
-        <v>7.4866666666666672</v>
+        <v>7.4084999999999992</v>
       </c>
       <c r="I27" s="1">
-        <v>7.5966666666666667</v>
+        <v>7.5004999999999979</v>
       </c>
       <c r="J27" s="1">
-        <v>7.6233333333333322</v>
+        <v>7.508</v>
       </c>
       <c r="K27" s="1">
-        <v>7.5866666666666669</v>
+        <v>7.5129999999999999</v>
       </c>
       <c r="L27" s="1">
-        <v>10</v>
+        <v>9.9664999999999999</v>
       </c>
       <c r="M27" s="1">
-        <v>10</v>
+        <v>9.9664999999999999</v>
       </c>
       <c r="N27" s="1">
-        <v>9.8883333333333336</v>
+        <v>9.9664999999999999</v>
       </c>
       <c r="O27" s="1">
-        <v>7.4849999999999994</v>
+        <v>7.4970000000000017</v>
       </c>
       <c r="P27" s="1">
-        <v>82.735000000000014</v>
+        <v>82.55149999999999</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>4</v>
@@ -2047,99 +2081,99 @@
       <c r="D28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="1">
-        <v>5.428881650380022E-2</v>
+      <c r="E28" s="4">
+        <v>2.8067993848015038</v>
       </c>
       <c r="F28" s="1">
-        <v>7.8900000000000006</v>
+        <v>7.5427272727272738</v>
       </c>
       <c r="G28" s="1">
-        <v>7.8066666666666675</v>
+        <v>7.4312121212121243</v>
       </c>
       <c r="H28" s="1">
-        <v>7.5266666666666664</v>
+        <v>7.2042424242424259</v>
       </c>
       <c r="I28" s="1">
-        <v>7.3900000000000006</v>
+        <v>7.5481818181818179</v>
       </c>
       <c r="J28" s="1">
-        <v>7.5533333333333337</v>
+        <v>7.3921212121212108</v>
       </c>
       <c r="K28" s="1">
-        <v>7.7233333333333336</v>
+        <v>7.4348484848484855</v>
       </c>
       <c r="L28" s="1">
-        <v>9.7766666666666655</v>
+        <v>9.9190909090909098</v>
       </c>
       <c r="M28" s="1">
-        <v>10</v>
+        <v>9.9796969696969686</v>
       </c>
       <c r="N28" s="1">
-        <v>10</v>
+        <v>9.9190909090909098</v>
       </c>
       <c r="O28" s="1">
-        <v>7.7233333333333336</v>
+        <v>7.2348484848484844</v>
       </c>
       <c r="P28" s="1">
-        <v>83.39</v>
+        <v>81.606060606060623</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="1">
-        <v>4.7075438390020014E-2</v>
+        <v>5</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2.7540743208888379</v>
       </c>
       <c r="F29" s="1">
-        <v>0</v>
+        <v>7.6037499999999998</v>
       </c>
       <c r="G29" s="1">
-        <v>7.8033333333333337</v>
+        <v>7.4175000000000004</v>
       </c>
       <c r="H29" s="1">
-        <v>7.9733333333333336</v>
+        <v>7.4587500000000002</v>
       </c>
       <c r="I29" s="1">
-        <v>8.0533333333333328</v>
+        <v>7.52</v>
       </c>
       <c r="J29" s="1">
-        <v>7.3633333333333333</v>
+        <v>7.5625</v>
       </c>
       <c r="K29" s="1">
-        <v>7.666666666666667</v>
+        <v>7.51</v>
       </c>
       <c r="L29" s="1">
-        <v>10</v>
+        <v>9.75</v>
       </c>
       <c r="M29" s="1">
-        <v>9.7766666666666655</v>
+        <v>9.75</v>
       </c>
       <c r="N29" s="1">
-        <v>9.7766666666666655</v>
+        <v>10</v>
       </c>
       <c r="O29" s="1">
-        <v>7.5266666666666664</v>
+        <v>7.7074999999999996</v>
       </c>
       <c r="P29" s="1">
-        <v>75.94</v>
+        <v>82.279999999999987</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>4</v>
@@ -2147,76 +2181,76 @@
       <c r="D30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="1">
-        <v>4.4205407794886908E-2</v>
+      <c r="E30" s="4">
+        <v>2.6308945271691981</v>
       </c>
       <c r="F30" s="1">
-        <v>7.625</v>
+        <v>7.1957142857142866</v>
       </c>
       <c r="G30" s="1">
-        <v>7.625</v>
+        <v>7.1143749999999999</v>
       </c>
       <c r="H30" s="1">
-        <v>7.415</v>
+        <v>7.0268750000000004</v>
       </c>
       <c r="I30" s="1">
-        <v>7.585</v>
+        <v>7.1931250000000002</v>
       </c>
       <c r="J30" s="1">
-        <v>7.665</v>
+        <v>7.1825000000000001</v>
       </c>
       <c r="K30" s="1">
-        <v>8.0449999999999999</v>
+        <v>7.0737500000000004</v>
       </c>
       <c r="L30" s="1">
-        <v>9.6649999999999991</v>
+        <v>9.458124999999999</v>
       </c>
       <c r="M30" s="1">
-        <v>9.6649999999999991</v>
+        <v>9.416875000000001</v>
       </c>
       <c r="N30" s="1">
-        <v>9.33</v>
+        <v>9.5</v>
       </c>
       <c r="O30" s="1">
-        <v>7.4550000000000001</v>
+        <v>7.1506249999999998</v>
       </c>
       <c r="P30" s="1">
-        <v>82.074999999999989</v>
+        <v>78.311964285714296</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="1">
-        <v>4.3061685865001614E-2</v>
+        <v>19</v>
+      </c>
+      <c r="E31" s="4">
+        <v>2.4496273098756332</v>
       </c>
       <c r="F31" s="1">
-        <v>7.833333333333333</v>
+        <v>7.4658333333333333</v>
       </c>
       <c r="G31" s="1">
-        <v>7.7766666666666664</v>
+        <v>7.3608333333333329</v>
       </c>
       <c r="H31" s="1">
-        <v>7.6099999999999994</v>
+        <v>7.1533333333333333</v>
       </c>
       <c r="I31" s="1">
-        <v>7.333333333333333</v>
+        <v>7.4183333333333339</v>
       </c>
       <c r="J31" s="1">
-        <v>7.78</v>
+        <v>7.34</v>
       </c>
       <c r="K31" s="1">
-        <v>7.75</v>
+        <v>7.2991666666666655</v>
       </c>
       <c r="L31" s="1">
         <v>10</v>
@@ -2225,48 +2259,48 @@
         <v>10</v>
       </c>
       <c r="N31" s="1">
-        <v>9.7766666666666655</v>
+        <v>10</v>
       </c>
       <c r="O31" s="1">
-        <v>7.6400000000000006</v>
+        <v>7.2975000000000003</v>
       </c>
       <c r="P31" s="1">
-        <v>83.5</v>
+        <v>81.334999999999994</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="1">
-        <v>0.41265132299654528</v>
+      <c r="E32" s="4">
+        <v>2.4393473572985829</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
       </c>
       <c r="G32" s="1">
-        <v>7.54</v>
+        <v>7.42</v>
       </c>
       <c r="H32" s="1">
-        <v>7.25</v>
+        <v>7.33</v>
       </c>
       <c r="I32" s="1">
-        <v>7.665</v>
+        <v>7.33</v>
       </c>
       <c r="J32" s="1">
-        <v>7.5</v>
+        <v>7.67</v>
       </c>
       <c r="K32" s="1">
-        <v>7.335</v>
+        <v>7.83</v>
       </c>
       <c r="L32" s="1">
         <v>10</v>
@@ -2278,10 +2312,10 @@
         <v>10</v>
       </c>
       <c r="O32" s="1">
-        <v>7.54</v>
+        <v>7.58</v>
       </c>
       <c r="P32" s="1">
-        <v>74.83</v>
+        <v>75.16</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -2289,334 +2323,334 @@
         <v>65</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="1">
-        <v>0.35627768960435324</v>
+        <v>13</v>
+      </c>
+      <c r="E33" s="4">
+        <v>2.4233534324773558</v>
       </c>
       <c r="F33" s="1">
-        <v>7.5427272727272738</v>
+        <v>0</v>
       </c>
       <c r="G33" s="1">
-        <v>7.4312121212121243</v>
+        <v>7.54</v>
       </c>
       <c r="H33" s="1">
-        <v>7.2042424242424259</v>
+        <v>7.25</v>
       </c>
       <c r="I33" s="1">
-        <v>7.5481818181818179</v>
+        <v>7.665</v>
       </c>
       <c r="J33" s="1">
-        <v>7.3921212121212108</v>
+        <v>7.5</v>
       </c>
       <c r="K33" s="1">
-        <v>7.4348484848484855</v>
+        <v>7.335</v>
       </c>
       <c r="L33" s="1">
-        <v>9.9190909090909098</v>
+        <v>10</v>
       </c>
       <c r="M33" s="1">
-        <v>9.9796969696969686</v>
+        <v>10</v>
       </c>
       <c r="N33" s="1">
-        <v>9.9190909090909098</v>
+        <v>10</v>
       </c>
       <c r="O33" s="1">
-        <v>7.2348484848484844</v>
+        <v>7.54</v>
       </c>
       <c r="P33" s="1">
-        <v>81.606060606060623</v>
+        <v>74.83</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="1">
-        <v>0.33743547893306797</v>
+        <v>11</v>
+      </c>
+      <c r="E34" s="4">
+        <v>2.3764474392803896</v>
       </c>
       <c r="F34" s="1">
-        <v>7.5151851851851852</v>
+        <v>7.4514285714285711</v>
       </c>
       <c r="G34" s="1">
-        <v>7.5188888888888874</v>
+        <v>7.4994999999999994</v>
       </c>
       <c r="H34" s="1">
-        <v>7.2774074074074075</v>
+        <v>7.4134999999999991</v>
       </c>
       <c r="I34" s="1">
-        <v>7.549999999999998</v>
+        <v>7.4000000000000012</v>
       </c>
       <c r="J34" s="1">
-        <v>7.4907407407407405</v>
+        <v>7.479000000000001</v>
       </c>
       <c r="K34" s="1">
-        <v>7.4759259259259245</v>
+        <v>7.4740000000000011</v>
       </c>
       <c r="L34" s="1">
-        <v>9.8022222222222233</v>
+        <v>9.9664999999999999</v>
       </c>
       <c r="M34" s="1">
-        <v>9.9011111111111134</v>
+        <v>9.7999999999999989</v>
       </c>
       <c r="N34" s="1">
-        <v>9.9011111111111134</v>
+        <v>9.7664999999999988</v>
       </c>
       <c r="O34" s="1">
-        <v>7.4940740740740752</v>
+        <v>7.4704999999999995</v>
       </c>
       <c r="P34" s="1">
-        <v>81.926666666666662</v>
+        <v>81.720928571428573</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="1">
-        <v>0.33413660511467708</v>
+        <v>61</v>
+      </c>
+      <c r="E35" s="4">
+        <v>2.3727742601273381</v>
       </c>
       <c r="F35" s="1">
-        <v>7.6385000000000005</v>
+        <v>7.4283333333333319</v>
       </c>
       <c r="G35" s="1">
-        <v>7.6289999999999996</v>
+        <v>7.6099999999999994</v>
       </c>
       <c r="H35" s="1">
-        <v>7.4164999999999992</v>
+        <v>7.5116666666666667</v>
       </c>
       <c r="I35" s="1">
-        <v>7.7410000000000014</v>
+        <v>7.6516666666666664</v>
       </c>
       <c r="J35" s="1">
-        <v>7.596000000000001</v>
+        <v>7.583333333333333</v>
       </c>
       <c r="K35" s="1">
-        <v>7.5205000000000002</v>
+        <v>7.6099999999999994</v>
       </c>
       <c r="L35" s="1">
-        <v>9.9330000000000016</v>
+        <v>10</v>
       </c>
       <c r="M35" s="1">
-        <v>9.9330000000000016</v>
+        <v>10</v>
       </c>
       <c r="N35" s="1">
-        <v>9.9330000000000016</v>
+        <v>10</v>
       </c>
       <c r="O35" s="1">
-        <v>7.5329999999999995</v>
+        <v>7.5683333333333325</v>
       </c>
       <c r="P35" s="1">
-        <v>82.873500000000007</v>
+        <v>82.963333333333324</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0.32511424930983229</v>
+        <v>9</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2.335784447431061</v>
       </c>
       <c r="F36" s="1">
-        <v>7.6219999999999999</v>
+        <v>8.0449999999999999</v>
       </c>
       <c r="G36" s="1">
-        <v>7.5837500000000002</v>
+        <v>7.835</v>
       </c>
       <c r="H36" s="1">
-        <v>7.2543749999999996</v>
+        <v>7.7050000000000001</v>
       </c>
       <c r="I36" s="1">
-        <v>7.6725000000000003</v>
+        <v>7.875</v>
       </c>
       <c r="J36" s="1">
-        <v>7.5006250000000003</v>
+        <v>8.125</v>
       </c>
       <c r="K36" s="1">
-        <v>7.4125000000000005</v>
+        <v>7.875</v>
       </c>
       <c r="L36" s="1">
-        <v>10</v>
+        <v>9.3350000000000009</v>
       </c>
       <c r="M36" s="1">
-        <v>10</v>
+        <v>9.6649999999999991</v>
       </c>
       <c r="N36" s="1">
-        <v>10</v>
+        <v>9.6649999999999991</v>
       </c>
       <c r="O36" s="1">
-        <v>7.375</v>
+        <v>7.75</v>
       </c>
       <c r="P36" s="1">
-        <v>82.420749999999998</v>
+        <v>83.875</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="1">
-        <v>0.29627306980011481</v>
+        <v>19</v>
+      </c>
+      <c r="E37" s="4">
+        <v>2.323463900026423</v>
       </c>
       <c r="F37" s="1">
-        <v>7.5670967741935486</v>
+        <v>7.6875</v>
       </c>
       <c r="G37" s="1">
-        <v>7.5196774193548359</v>
+        <v>7.7074999999999996</v>
       </c>
       <c r="H37" s="1">
-        <v>7.2638709677419353</v>
+        <v>7.6875</v>
       </c>
       <c r="I37" s="1">
-        <v>7.6183870967741942</v>
+        <v>7.585</v>
       </c>
       <c r="J37" s="1">
-        <v>7.4490322580645136</v>
+        <v>7.8125</v>
       </c>
       <c r="K37" s="1">
-        <v>7.4822580645161256</v>
+        <v>7.73</v>
       </c>
       <c r="L37" s="1">
-        <v>9.8706451612903212</v>
+        <v>10</v>
       </c>
       <c r="M37" s="1">
-        <v>9.9351612903225792</v>
+        <v>10</v>
       </c>
       <c r="N37" s="1">
-        <v>9.9567741935483856</v>
+        <v>10</v>
       </c>
       <c r="O37" s="1">
-        <v>7.4009677419354833</v>
+        <v>7.875</v>
       </c>
       <c r="P37" s="1">
-        <v>82.06387096774192</v>
+        <v>84.085000000000008</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="1">
-        <v>0.27283701457015164</v>
+        <v>43</v>
+      </c>
+      <c r="E38" s="4">
+        <v>2.2983719547305244</v>
       </c>
       <c r="F38" s="1">
-        <v>7.4843478260869585</v>
+        <v>0</v>
       </c>
       <c r="G38" s="1">
-        <v>7.3839130434782616</v>
+        <v>7.4553333333333329</v>
       </c>
       <c r="H38" s="1">
-        <v>7.2078260869565254</v>
+        <v>7.3493333333333339</v>
       </c>
       <c r="I38" s="1">
-        <v>7.5452173913043472</v>
+        <v>7.4993333333333334</v>
       </c>
       <c r="J38" s="1">
-        <v>7.4528260869565202</v>
+        <v>7.5</v>
       </c>
       <c r="K38" s="1">
-        <v>7.463043478260869</v>
+        <v>7.3386666666666667</v>
       </c>
       <c r="L38" s="1">
-        <v>9.7391304347826093</v>
+        <v>9.4666666666666668</v>
       </c>
       <c r="M38" s="1">
-        <v>9.7099999999999991</v>
+        <v>9.4666666666666668</v>
       </c>
       <c r="N38" s="1">
-        <v>9.6663043478260864</v>
+        <v>10</v>
       </c>
       <c r="O38" s="1">
-        <v>7.3393478260869554</v>
+        <v>7.4613333333333332</v>
       </c>
       <c r="P38" s="1">
-        <v>80.991956521739141</v>
+        <v>73.537333333333322</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0.21312882399908734</v>
+        <v>27</v>
+      </c>
+      <c r="E39" s="4">
+        <v>2.2893581456910317</v>
       </c>
       <c r="F39" s="1">
-        <v>0</v>
+        <v>8.2949999999999999</v>
       </c>
       <c r="G39" s="1">
-        <v>6.5</v>
+        <v>7.92</v>
       </c>
       <c r="H39" s="1">
-        <v>6.5</v>
+        <v>7.96</v>
       </c>
       <c r="I39" s="1">
-        <v>7.17</v>
+        <v>7.75</v>
       </c>
       <c r="J39" s="1">
-        <v>7</v>
+        <v>8.125</v>
       </c>
       <c r="K39" s="1">
-        <v>6.83</v>
+        <v>8</v>
       </c>
       <c r="L39" s="1">
         <v>10</v>
@@ -2628,110 +2662,110 @@
         <v>10</v>
       </c>
       <c r="O39" s="1">
-        <v>6.17</v>
+        <v>8.125</v>
       </c>
       <c r="P39" s="1">
-        <v>70.17</v>
+        <v>86.174999999999997</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0.53888579012628635</v>
+        <v>9</v>
+      </c>
+      <c r="E40" s="4">
+        <v>2.2722964870236231</v>
       </c>
       <c r="F40" s="1">
-        <v>7.5</v>
+        <v>7.6479999999999988</v>
       </c>
       <c r="G40" s="1">
-        <v>7.42</v>
+        <v>7.5840000000000005</v>
       </c>
       <c r="H40" s="1">
-        <v>7.08</v>
+        <v>7.6319999999999997</v>
       </c>
       <c r="I40" s="1">
-        <v>7.42</v>
+        <v>7.7680000000000007</v>
       </c>
       <c r="J40" s="1">
-        <v>7.5</v>
+        <v>7.5820000000000007</v>
       </c>
       <c r="K40" s="1">
-        <v>7.33</v>
+        <v>7.6340000000000003</v>
       </c>
       <c r="L40" s="1">
-        <v>10</v>
+        <v>9.734</v>
       </c>
       <c r="M40" s="1">
-        <v>10</v>
+        <v>9.734</v>
       </c>
       <c r="N40" s="1">
-        <v>10</v>
+        <v>9.7319999999999993</v>
       </c>
       <c r="O40" s="1">
-        <v>7.33</v>
+        <v>7.7180000000000009</v>
       </c>
       <c r="P40" s="1">
-        <v>81.58</v>
+        <v>82.766000000000005</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E41" s="1">
-        <v>0.49864655766155197</v>
+        <v>11</v>
+      </c>
+      <c r="E41" s="4">
+        <v>2.2615443428999553</v>
       </c>
       <c r="F41" s="1">
-        <v>6.84</v>
+        <v>7.4275000000000002</v>
       </c>
       <c r="G41" s="1">
-        <v>6.8172727272727265</v>
+        <v>7.5512500000000005</v>
       </c>
       <c r="H41" s="1">
-        <v>6.5909090909090908</v>
+        <v>7.46875</v>
       </c>
       <c r="I41" s="1">
-        <v>6.7654545454545456</v>
+        <v>7.6050000000000004</v>
       </c>
       <c r="J41" s="1">
-        <v>6.7427272727272731</v>
+        <v>7.4799999999999995</v>
       </c>
       <c r="K41" s="1">
-        <v>6.6972727272727273</v>
+        <v>7.5325000000000006</v>
       </c>
       <c r="L41" s="1">
-        <v>9.0909090909090917</v>
+        <v>9.9162499999999998</v>
       </c>
       <c r="M41" s="1">
-        <v>9.0909090909090917</v>
+        <v>10</v>
       </c>
       <c r="N41" s="1">
-        <v>9.0909090909090917</v>
+        <v>10</v>
       </c>
       <c r="O41" s="1">
-        <v>6.7345454545454544</v>
+        <v>7.5625</v>
       </c>
       <c r="P41" s="1">
-        <v>74.460909090909098</v>
+        <v>82.543749999999989</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -2739,34 +2773,34 @@
         <v>34</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0.48536952792459975</v>
+        <v>5</v>
+      </c>
+      <c r="E42" s="4">
+        <v>2.2472485146595389</v>
       </c>
       <c r="F42" s="1">
-        <v>7.6022222222222222</v>
+        <v>7.5</v>
       </c>
       <c r="G42" s="1">
-        <v>7.6340000000000003</v>
+        <v>7.5</v>
       </c>
       <c r="H42" s="1">
-        <v>7.4159999999999995</v>
+        <v>7.5</v>
       </c>
       <c r="I42" s="1">
-        <v>7.5010000000000003</v>
+        <v>7.67</v>
       </c>
       <c r="J42" s="1">
-        <v>7.6260000000000003</v>
+        <v>7.67</v>
       </c>
       <c r="K42" s="1">
-        <v>7.5250000000000004</v>
+        <v>7.67</v>
       </c>
       <c r="L42" s="1">
         <v>10</v>
@@ -2778,45 +2812,45 @@
         <v>10</v>
       </c>
       <c r="O42" s="1">
-        <v>7.4899999999999993</v>
+        <v>7.67</v>
       </c>
       <c r="P42" s="1">
-        <v>82.794222222222217</v>
+        <v>83.18</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="1">
-        <v>0.44498861317592259</v>
+        <v>43</v>
+      </c>
+      <c r="E43" s="4">
+        <v>2.217214191415994</v>
       </c>
       <c r="F43" s="1">
-        <v>7.5</v>
+        <v>7.7766666666666664</v>
       </c>
       <c r="G43" s="1">
-        <v>7.5</v>
+        <v>7.6320000000000006</v>
       </c>
       <c r="H43" s="1">
-        <v>7.5</v>
+        <v>7.516</v>
       </c>
       <c r="I43" s="1">
-        <v>7.67</v>
+        <v>7.548</v>
       </c>
       <c r="J43" s="1">
-        <v>7.67</v>
+        <v>7.6820000000000004</v>
       </c>
       <c r="K43" s="1">
-        <v>7.67</v>
+        <v>7.831999999999999</v>
       </c>
       <c r="L43" s="1">
         <v>10</v>
@@ -2828,248 +2862,248 @@
         <v>10</v>
       </c>
       <c r="O43" s="1">
-        <v>7.67</v>
+        <v>7.65</v>
       </c>
       <c r="P43" s="1">
-        <v>83.18</v>
+        <v>83.636666666666684</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="1">
-        <v>0.4082253639027113</v>
+        <v>11</v>
+      </c>
+      <c r="E44" s="4">
+        <v>2.2111315271237051</v>
       </c>
       <c r="F44" s="1">
-        <v>7.4658333333333333</v>
+        <v>7.42</v>
       </c>
       <c r="G44" s="1">
-        <v>7.3608333333333329</v>
+        <v>7.75</v>
       </c>
       <c r="H44" s="1">
-        <v>7.1533333333333333</v>
+        <v>7.42</v>
       </c>
       <c r="I44" s="1">
-        <v>7.4183333333333339</v>
+        <v>7.67</v>
       </c>
       <c r="J44" s="1">
-        <v>7.34</v>
+        <v>7.92</v>
       </c>
       <c r="K44" s="1">
-        <v>7.2991666666666655</v>
+        <v>7.83</v>
       </c>
       <c r="L44" s="1">
-        <v>10</v>
+        <v>8.67</v>
       </c>
       <c r="M44" s="1">
-        <v>10</v>
+        <v>5.33</v>
       </c>
       <c r="N44" s="1">
-        <v>10</v>
+        <v>9.33</v>
       </c>
       <c r="O44" s="1">
-        <v>7.2975000000000003</v>
+        <v>7.67</v>
       </c>
       <c r="P44" s="1">
-        <v>81.334999999999994</v>
+        <v>77.010000000000005</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0.38009885598720095</v>
+        <v>5</v>
+      </c>
+      <c r="E45" s="4">
+        <v>2.1949999999999998</v>
       </c>
       <c r="F45" s="1">
-        <v>7.1957142857142866</v>
+        <v>7.5</v>
       </c>
       <c r="G45" s="1">
-        <v>7.1143749999999999</v>
+        <v>7.67</v>
       </c>
       <c r="H45" s="1">
-        <v>7.0268750000000004</v>
+        <v>7.58</v>
       </c>
       <c r="I45" s="1">
-        <v>7.1931250000000002</v>
+        <v>7.75</v>
       </c>
       <c r="J45" s="1">
-        <v>7.1825000000000001</v>
+        <v>7.83</v>
       </c>
       <c r="K45" s="1">
-        <v>7.0737500000000004</v>
+        <v>7.83</v>
       </c>
       <c r="L45" s="1">
-        <v>9.458124999999999</v>
+        <v>10</v>
       </c>
       <c r="M45" s="1">
-        <v>9.416875000000001</v>
+        <v>10</v>
       </c>
       <c r="N45" s="1">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="O45" s="1">
-        <v>7.1506249999999998</v>
+        <v>7.67</v>
       </c>
       <c r="P45" s="1">
-        <v>78.311964285714296</v>
+        <v>83.83</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="1">
-        <v>0.32154515422211266</v>
+        <v>17</v>
+      </c>
+      <c r="E46" s="4">
+        <v>2.1913911498346406</v>
       </c>
       <c r="F46" s="1">
-        <v>7.335</v>
+        <v>7.4627777777777773</v>
       </c>
       <c r="G46" s="1">
-        <v>7.5</v>
+        <v>7.4485714285714284</v>
       </c>
       <c r="H46" s="1">
-        <v>7.375</v>
+        <v>7.4090476190476195</v>
       </c>
       <c r="I46" s="1">
-        <v>7.375</v>
+        <v>7.4804761904761907</v>
       </c>
       <c r="J46" s="1">
-        <v>7.54</v>
+        <v>7.4719047619047627</v>
       </c>
       <c r="K46" s="1">
-        <v>7.5</v>
+        <v>7.3971428571428559</v>
       </c>
       <c r="L46" s="1">
-        <v>10</v>
+        <v>9.8409523809523822</v>
       </c>
       <c r="M46" s="1">
-        <v>10</v>
+        <v>9.9047619047619051</v>
       </c>
       <c r="N46" s="1">
-        <v>10</v>
+        <v>9.9680952380952395</v>
       </c>
       <c r="O46" s="1">
-        <v>7.5449999999999999</v>
+        <v>7.5433333333333321</v>
       </c>
       <c r="P46" s="1">
-        <v>82.17</v>
+        <v>81.927063492063496</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="1">
-        <v>1.4407205225330244</v>
+        <v>17</v>
+      </c>
+      <c r="E47" s="4">
+        <v>2.1739163368105001</v>
       </c>
       <c r="F47" s="1">
-        <v>7.3866666666666667</v>
+        <v>7.6574074074074074</v>
       </c>
       <c r="G47" s="1">
-        <v>7.2233333333333336</v>
+        <v>7.6574074074074074</v>
       </c>
       <c r="H47" s="1">
-        <v>7.1400000000000006</v>
+        <v>7.5637037037037045</v>
       </c>
       <c r="I47" s="1">
-        <v>7.1400000000000006</v>
+        <v>7.5899999999999972</v>
       </c>
       <c r="J47" s="1">
-        <v>7.3900000000000006</v>
+        <v>7.623703703703705</v>
       </c>
       <c r="K47" s="1">
-        <v>7.4466666666666663</v>
+        <v>7.7455555555555575</v>
       </c>
       <c r="L47" s="1">
-        <v>10</v>
+        <v>9.975185185185186</v>
       </c>
       <c r="M47" s="1">
-        <v>10</v>
+        <v>9.975185185185186</v>
       </c>
       <c r="N47" s="1">
         <v>10</v>
       </c>
       <c r="O47" s="1">
-        <v>7.246666666666667</v>
+        <v>7.6629629629629621</v>
       </c>
       <c r="P47" s="1">
-        <v>80.973333333333329</v>
+        <v>83.451111111111103</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="1">
-        <v>0.79853883249487823</v>
+        <v>19</v>
+      </c>
+      <c r="E48" s="4">
+        <v>2.0911466630518341</v>
       </c>
       <c r="F48" s="1">
-        <v>6.83</v>
+        <v>7.7953333333333328</v>
       </c>
       <c r="G48" s="1">
-        <v>7.125</v>
+        <v>7.6970000000000001</v>
       </c>
       <c r="H48" s="1">
-        <v>7.0449999999999999</v>
+        <v>7.6570000000000009</v>
       </c>
       <c r="I48" s="1">
-        <v>6.835</v>
+        <v>7.7080000000000002</v>
       </c>
       <c r="J48" s="1">
-        <v>7.375</v>
+        <v>7.7580000000000009</v>
       </c>
       <c r="K48" s="1">
-        <v>7.08</v>
+        <v>7.7209999999999992</v>
       </c>
       <c r="L48" s="1">
-        <v>10</v>
+        <v>9.833499999999999</v>
       </c>
       <c r="M48" s="1">
         <v>10</v>
@@ -3078,368 +3112,368 @@
         <v>10</v>
       </c>
       <c r="O48" s="1">
-        <v>6.92</v>
+        <v>7.6709999999999994</v>
       </c>
       <c r="P48" s="1">
-        <v>79.209999999999994</v>
+        <v>83.840833333333336</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E49" s="1">
-        <v>0.79653345878988457</v>
+        <v>17</v>
+      </c>
+      <c r="E49" s="4">
+        <v>2.0602859109757419</v>
       </c>
       <c r="F49" s="1">
-        <v>0</v>
+        <v>7.6022222222222222</v>
       </c>
       <c r="G49" s="1">
-        <v>7.7050000000000001</v>
+        <v>7.6340000000000003</v>
       </c>
       <c r="H49" s="1">
-        <v>7.665</v>
+        <v>7.4159999999999995</v>
       </c>
       <c r="I49" s="1">
-        <v>7.875</v>
+        <v>7.5010000000000003</v>
       </c>
       <c r="J49" s="1">
-        <v>7.835</v>
+        <v>7.6260000000000003</v>
       </c>
       <c r="K49" s="1">
-        <v>7.875</v>
+        <v>7.5250000000000004</v>
       </c>
       <c r="L49" s="1">
-        <v>9.6649999999999991</v>
+        <v>10</v>
       </c>
       <c r="M49" s="1">
-        <v>9.6649999999999991</v>
+        <v>10</v>
       </c>
       <c r="N49" s="1">
-        <v>9.6649999999999991</v>
+        <v>10</v>
       </c>
       <c r="O49" s="1">
-        <v>8.2100000000000009</v>
+        <v>7.4899999999999993</v>
       </c>
       <c r="P49" s="1">
-        <v>76.16</v>
+        <v>82.794222222222217</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="1">
-        <v>0.83826546540804203</v>
+        <v>5</v>
+      </c>
+      <c r="E50" s="4">
+        <v>2.0498147447864996</v>
       </c>
       <c r="F50" s="1">
-        <v>8.33</v>
+        <v>7.6475000000000009</v>
       </c>
       <c r="G50" s="1">
-        <v>8.42</v>
+        <v>7.5670000000000002</v>
       </c>
       <c r="H50" s="1">
-        <v>7.83</v>
+        <v>7.4510000000000005</v>
       </c>
       <c r="I50" s="1">
-        <v>8.33</v>
+        <v>7.5250000000000004</v>
       </c>
       <c r="J50" s="1">
-        <v>8</v>
+        <v>7.660000000000001</v>
       </c>
       <c r="K50" s="1">
-        <v>8.25</v>
+        <v>7.6669999999999998</v>
       </c>
       <c r="L50" s="1">
-        <v>9.33</v>
+        <v>9.9329999999999998</v>
       </c>
       <c r="M50" s="1">
-        <v>9.33</v>
+        <v>9.9329999999999998</v>
       </c>
       <c r="N50" s="1">
         <v>10</v>
       </c>
       <c r="O50" s="1">
-        <v>7.92</v>
+        <v>7.6340000000000003</v>
       </c>
       <c r="P50" s="1">
-        <v>85.74</v>
+        <v>83.017499999999998</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="1">
-        <v>0.57528013328048899</v>
+        <v>43</v>
+      </c>
+      <c r="E51" s="4">
+        <v>2.0054284635786721</v>
       </c>
       <c r="F51" s="1">
-        <v>7.5659999999999998</v>
+        <v>6.84</v>
       </c>
       <c r="G51" s="1">
-        <v>7.5659999999999998</v>
+        <v>6.8172727272727265</v>
       </c>
       <c r="H51" s="1">
-        <v>7.4659999999999993</v>
+        <v>6.5909090909090908</v>
       </c>
       <c r="I51" s="1">
-        <v>7.6480000000000006</v>
+        <v>6.7654545454545456</v>
       </c>
       <c r="J51" s="1">
-        <v>7.6519999999999992</v>
+        <v>6.7427272727272731</v>
       </c>
       <c r="K51" s="1">
-        <v>7.55</v>
+        <v>6.6972727272727273</v>
       </c>
       <c r="L51" s="1">
-        <v>9.597999999999999</v>
+        <v>9.0909090909090917</v>
       </c>
       <c r="M51" s="1">
-        <v>10</v>
+        <v>9.0909090909090917</v>
       </c>
       <c r="N51" s="1">
-        <v>10</v>
+        <v>9.0909090909090917</v>
       </c>
       <c r="O51" s="1">
-        <v>7.484</v>
+        <v>6.7345454545454544</v>
       </c>
       <c r="P51" s="1">
-        <v>82.529999999999987</v>
+        <v>74.460909090909098</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="1">
-        <v>0.4522571306740964</v>
+        <v>5</v>
+      </c>
+      <c r="E52" s="4">
+        <v>2.0026297005585172</v>
       </c>
       <c r="F52" s="1">
-        <v>7.42</v>
+        <v>7.6492500000000021</v>
       </c>
       <c r="G52" s="1">
-        <v>7.75</v>
+        <v>7.5567499999999983</v>
       </c>
       <c r="H52" s="1">
-        <v>7.42</v>
+        <v>7.5187499999999998</v>
       </c>
       <c r="I52" s="1">
-        <v>7.67</v>
+        <v>7.5667500000000008</v>
       </c>
       <c r="J52" s="1">
-        <v>7.92</v>
+        <v>7.5975000000000037</v>
       </c>
       <c r="K52" s="1">
-        <v>7.83</v>
+        <v>7.7082500000000014</v>
       </c>
       <c r="L52" s="1">
-        <v>8.67</v>
+        <v>9.9</v>
       </c>
       <c r="M52" s="1">
-        <v>5.33</v>
+        <v>9.8167500000000008</v>
       </c>
       <c r="N52" s="1">
-        <v>9.33</v>
+        <v>9.9167500000000004</v>
       </c>
       <c r="O52" s="1">
-        <v>7.67</v>
+        <v>7.625</v>
       </c>
       <c r="P52" s="1">
-        <v>77.010000000000005</v>
+        <v>82.85575</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="1">
-        <v>0.42812169637477404</v>
+        <v>5</v>
+      </c>
+      <c r="E53" s="4">
+        <v>1.9792914837122431</v>
       </c>
       <c r="F53" s="1">
-        <v>8.0449999999999999</v>
+        <v>6.75</v>
       </c>
       <c r="G53" s="1">
-        <v>7.835</v>
+        <v>6.67</v>
       </c>
       <c r="H53" s="1">
-        <v>7.7050000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="I53" s="1">
-        <v>7.875</v>
+        <v>6.83</v>
       </c>
       <c r="J53" s="1">
-        <v>8.125</v>
+        <v>6.67</v>
       </c>
       <c r="K53" s="1">
-        <v>7.875</v>
+        <v>6.92</v>
       </c>
       <c r="L53" s="1">
-        <v>9.3350000000000009</v>
+        <v>9.33</v>
       </c>
       <c r="M53" s="1">
-        <v>9.6649999999999991</v>
+        <v>9.33</v>
       </c>
       <c r="N53" s="1">
-        <v>9.6649999999999991</v>
+        <v>6.83</v>
       </c>
       <c r="O53" s="1">
-        <v>7.75</v>
+        <v>7.92</v>
       </c>
       <c r="P53" s="1">
-        <v>83.875</v>
+        <v>73.75</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="1">
-        <v>0.32192258864941548</v>
+        <v>19</v>
+      </c>
+      <c r="E54" s="4">
+        <v>1.9421207394673226</v>
       </c>
       <c r="F54" s="1">
-        <v>6.83</v>
+        <v>7.5485714285714289</v>
       </c>
       <c r="G54" s="1">
-        <v>6.5</v>
+        <v>7.5545833333333343</v>
       </c>
       <c r="H54" s="1">
-        <v>6.5</v>
+        <v>7.3641666666666659</v>
       </c>
       <c r="I54" s="1">
-        <v>6.92</v>
+        <v>7.4754166666666668</v>
       </c>
       <c r="J54" s="1">
-        <v>6.75</v>
+        <v>7.5379166666666668</v>
       </c>
       <c r="K54" s="1">
-        <v>7</v>
+        <v>7.5870833333333332</v>
       </c>
       <c r="L54" s="1">
-        <v>9.33</v>
+        <v>9.9720833333333339</v>
       </c>
       <c r="M54" s="1">
-        <v>10</v>
+        <v>9.8612500000000001</v>
       </c>
       <c r="N54" s="1">
-        <v>9.33</v>
+        <v>10</v>
       </c>
       <c r="O54" s="1">
-        <v>6.67</v>
+        <v>7.5691666666666686</v>
       </c>
       <c r="P54" s="1">
-        <v>75.83</v>
+        <v>82.470238095238102</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E55" s="1">
-        <v>0.446891250769481</v>
+      <c r="E55" s="4">
+        <v>1.9203487418041596</v>
       </c>
       <c r="F55" s="1">
-        <v>7.4275000000000002</v>
+        <v>7.8659999999999997</v>
       </c>
       <c r="G55" s="1">
-        <v>7.5512500000000005</v>
+        <v>7.8340000000000005</v>
       </c>
       <c r="H55" s="1">
-        <v>7.46875</v>
+        <v>7.7319999999999993</v>
       </c>
       <c r="I55" s="1">
-        <v>7.6050000000000004</v>
+        <v>7.7</v>
       </c>
       <c r="J55" s="1">
-        <v>7.4799999999999995</v>
+        <v>7.6819999999999995</v>
       </c>
       <c r="K55" s="1">
-        <v>7.5325000000000006</v>
+        <v>7.7180000000000009</v>
       </c>
       <c r="L55" s="1">
-        <v>9.9162499999999998</v>
+        <v>10</v>
       </c>
       <c r="M55" s="1">
         <v>10</v>
       </c>
       <c r="N55" s="1">
-        <v>10</v>
+        <v>8.6</v>
       </c>
       <c r="O55" s="1">
-        <v>7.5625</v>
+        <v>7.831999999999999</v>
       </c>
       <c r="P55" s="1">
-        <v>82.543749999999989</v>
+        <v>82.963999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>8</v>
@@ -3447,76 +3481,76 @@
       <c r="D56" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E56" s="1">
-        <v>0.44008341592335698</v>
+      <c r="E56" s="4">
+        <v>1.9007217847769029</v>
       </c>
       <c r="F56" s="1">
-        <v>7.6479999999999988</v>
+        <v>7.67</v>
       </c>
       <c r="G56" s="1">
-        <v>7.5840000000000005</v>
+        <v>7.665</v>
       </c>
       <c r="H56" s="1">
-        <v>7.6319999999999997</v>
+        <v>7.17</v>
       </c>
       <c r="I56" s="1">
-        <v>7.7680000000000007</v>
+        <v>7.33</v>
       </c>
       <c r="J56" s="1">
-        <v>7.5820000000000007</v>
+        <v>7.875</v>
       </c>
       <c r="K56" s="1">
-        <v>7.6340000000000003</v>
+        <v>7.25</v>
       </c>
       <c r="L56" s="1">
-        <v>9.734</v>
+        <v>10</v>
       </c>
       <c r="M56" s="1">
-        <v>9.734</v>
+        <v>10</v>
       </c>
       <c r="N56" s="1">
-        <v>9.7319999999999993</v>
+        <v>10</v>
       </c>
       <c r="O56" s="1">
-        <v>7.7180000000000009</v>
+        <v>7.5449999999999999</v>
       </c>
       <c r="P56" s="1">
-        <v>82.766000000000005</v>
+        <v>82.50500000000001</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="1">
-        <v>0.43742977159411889</v>
+        <v>35</v>
+      </c>
+      <c r="E57" s="4">
+        <v>1.8556807737788981</v>
       </c>
       <c r="F57" s="1">
-        <v>7.6875</v>
+        <v>7.5</v>
       </c>
       <c r="G57" s="1">
-        <v>7.7074999999999996</v>
+        <v>7.42</v>
       </c>
       <c r="H57" s="1">
-        <v>7.6875</v>
+        <v>7.08</v>
       </c>
       <c r="I57" s="1">
-        <v>7.585</v>
+        <v>7.42</v>
       </c>
       <c r="J57" s="1">
-        <v>7.8125</v>
+        <v>7.5</v>
       </c>
       <c r="K57" s="1">
-        <v>7.73</v>
+        <v>7.33</v>
       </c>
       <c r="L57" s="1">
         <v>10</v>
@@ -3528,45 +3562,45 @@
         <v>10</v>
       </c>
       <c r="O57" s="1">
-        <v>7.875</v>
+        <v>7.33</v>
       </c>
       <c r="P57" s="1">
-        <v>84.085000000000008</v>
+        <v>81.58</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E58" s="1">
-        <v>0.42144759272057081</v>
+        <v>9</v>
+      </c>
+      <c r="E58" s="4">
+        <v>1.818347761902289</v>
       </c>
       <c r="F58" s="1">
-        <v>7.4283333333333319</v>
+        <v>8.0180000000000007</v>
       </c>
       <c r="G58" s="1">
-        <v>7.6099999999999994</v>
+        <v>7.8159999999999998</v>
       </c>
       <c r="H58" s="1">
-        <v>7.5116666666666667</v>
+        <v>7.6480000000000006</v>
       </c>
       <c r="I58" s="1">
-        <v>7.6516666666666664</v>
+        <v>7.8340000000000005</v>
       </c>
       <c r="J58" s="1">
-        <v>7.583333333333333</v>
+        <v>7.8</v>
       </c>
       <c r="K58" s="1">
-        <v>7.6099999999999994</v>
+        <v>7.766</v>
       </c>
       <c r="L58" s="1">
         <v>10</v>
@@ -3578,48 +3612,48 @@
         <v>10</v>
       </c>
       <c r="O58" s="1">
-        <v>7.5683333333333325</v>
+        <v>7.734</v>
       </c>
       <c r="P58" s="1">
-        <v>82.963333333333324</v>
+        <v>84.616</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E59" s="1">
-        <v>0.32878433457413803</v>
+      <c r="E59" s="4">
+        <v>1.7382835633443141</v>
       </c>
       <c r="F59" s="1">
-        <v>7.2925000000000004</v>
+        <v>7.5659999999999998</v>
       </c>
       <c r="G59" s="1">
-        <v>7.3125</v>
+        <v>7.5659999999999998</v>
       </c>
       <c r="H59" s="1">
-        <v>7.1675000000000004</v>
+        <v>7.4659999999999993</v>
       </c>
       <c r="I59" s="1">
-        <v>7.5024999999999995</v>
+        <v>7.6480000000000006</v>
       </c>
       <c r="J59" s="1">
-        <v>7.2900000000000009</v>
+        <v>7.6519999999999992</v>
       </c>
       <c r="K59" s="1">
-        <v>7.23</v>
+        <v>7.55</v>
       </c>
       <c r="L59" s="1">
-        <v>10</v>
+        <v>9.597999999999999</v>
       </c>
       <c r="M59" s="1">
         <v>10</v>
@@ -3628,10 +3662,10 @@
         <v>10</v>
       </c>
       <c r="O59" s="1">
-        <v>7.2274999999999991</v>
+        <v>7.484</v>
       </c>
       <c r="P59" s="1">
-        <v>81.022500000000008</v>
+        <v>82.529999999999987</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -3639,34 +3673,34 @@
         <v>15</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E60" s="1">
-        <v>0.70042105368702967</v>
+        <v>19</v>
+      </c>
+      <c r="E60" s="4">
+        <v>1.5483026833204945</v>
       </c>
       <c r="F60" s="1">
-        <v>8.0449999999999999</v>
+        <v>7.6050000000000004</v>
       </c>
       <c r="G60" s="1">
-        <v>7.835</v>
+        <v>7.6675000000000004</v>
       </c>
       <c r="H60" s="1">
-        <v>7.71</v>
+        <v>7.48</v>
       </c>
       <c r="I60" s="1">
-        <v>7.75</v>
+        <v>7.5425000000000004</v>
       </c>
       <c r="J60" s="1">
-        <v>7.75</v>
+        <v>7.6475000000000009</v>
       </c>
       <c r="K60" s="1">
-        <v>7.75</v>
+        <v>7.5625</v>
       </c>
       <c r="L60" s="1">
         <v>10</v>
@@ -3678,10 +3712,10 @@
         <v>10</v>
       </c>
       <c r="O60" s="1">
-        <v>7.915</v>
+        <v>7.6675000000000004</v>
       </c>
       <c r="P60" s="1">
-        <v>84.75500000000001</v>
+        <v>83.172499999999999</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -3689,34 +3723,34 @@
         <v>15</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E61" s="1">
-        <v>0.66009757809172753</v>
+        <v>5</v>
+      </c>
+      <c r="E61" s="4">
+        <v>1.5204875310987109</v>
       </c>
       <c r="F61" s="1">
-        <v>7.6050000000000004</v>
+        <v>7.8950000000000014</v>
       </c>
       <c r="G61" s="1">
-        <v>7.6675000000000004</v>
+        <v>7.7255000000000011</v>
       </c>
       <c r="H61" s="1">
-        <v>7.48</v>
+        <v>7.6085000000000012</v>
       </c>
       <c r="I61" s="1">
-        <v>7.5425000000000004</v>
+        <v>7.7085000000000008</v>
       </c>
       <c r="J61" s="1">
-        <v>7.6475000000000009</v>
+        <v>7.6744999999999992</v>
       </c>
       <c r="K61" s="1">
-        <v>7.5625</v>
+        <v>7.7009999999999987</v>
       </c>
       <c r="L61" s="1">
         <v>10</v>
@@ -3725,63 +3759,63 @@
         <v>10</v>
       </c>
       <c r="N61" s="1">
-        <v>10</v>
+        <v>9.1834999999999987</v>
       </c>
       <c r="O61" s="1">
-        <v>7.6675000000000004</v>
+        <v>7.7129999999999992</v>
       </c>
       <c r="P61" s="1">
-        <v>83.172499999999999</v>
+        <v>83.209500000000006</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" s="1">
-        <v>0.65787277821280599</v>
+        <v>9</v>
+      </c>
+      <c r="E62" s="4">
+        <v>1.500773079009996</v>
       </c>
       <c r="F62" s="1">
-        <v>7.8950000000000014</v>
+        <v>8.33</v>
       </c>
       <c r="G62" s="1">
-        <v>7.7255000000000011</v>
+        <v>8.42</v>
       </c>
       <c r="H62" s="1">
-        <v>7.6085000000000012</v>
+        <v>7.83</v>
       </c>
       <c r="I62" s="1">
-        <v>7.7085000000000008</v>
+        <v>8.33</v>
       </c>
       <c r="J62" s="1">
-        <v>7.6744999999999992</v>
+        <v>8</v>
       </c>
       <c r="K62" s="1">
-        <v>7.7009999999999987</v>
+        <v>8.25</v>
       </c>
       <c r="L62" s="1">
-        <v>10</v>
+        <v>9.33</v>
       </c>
       <c r="M62" s="1">
-        <v>10</v>
+        <v>9.33</v>
       </c>
       <c r="N62" s="1">
-        <v>9.1834999999999987</v>
+        <v>10</v>
       </c>
       <c r="O62" s="1">
-        <v>7.7129999999999992</v>
+        <v>7.92</v>
       </c>
       <c r="P62" s="1">
-        <v>83.209500000000006</v>
+        <v>85.74</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
@@ -3789,34 +3823,34 @@
         <v>15</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="1">
-        <v>0.55939155162615617</v>
+        <v>17</v>
+      </c>
+      <c r="E63" s="4">
+        <v>1.4394080684924111</v>
       </c>
       <c r="F63" s="1">
-        <v>8.0180000000000007</v>
+        <v>8.0449999999999999</v>
       </c>
       <c r="G63" s="1">
-        <v>7.8159999999999998</v>
+        <v>7.835</v>
       </c>
       <c r="H63" s="1">
-        <v>7.6480000000000006</v>
+        <v>7.71</v>
       </c>
       <c r="I63" s="1">
-        <v>7.8340000000000005</v>
+        <v>7.75</v>
       </c>
       <c r="J63" s="1">
-        <v>7.8</v>
+        <v>7.75</v>
       </c>
       <c r="K63" s="1">
-        <v>7.766</v>
+        <v>7.75</v>
       </c>
       <c r="L63" s="1">
         <v>10</v>
@@ -3828,95 +3862,95 @@
         <v>10</v>
       </c>
       <c r="O63" s="1">
-        <v>7.734</v>
+        <v>7.915</v>
       </c>
       <c r="P63" s="1">
-        <v>84.616</v>
+        <v>84.75500000000001</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="1">
-        <v>0.5409854273326492</v>
+        <v>13</v>
+      </c>
+      <c r="E64" s="4">
+        <v>1.255440043308699</v>
       </c>
       <c r="F64" s="1">
-        <v>7.8659999999999997</v>
+        <v>0</v>
       </c>
       <c r="G64" s="1">
-        <v>7.8340000000000005</v>
+        <v>7.7050000000000001</v>
       </c>
       <c r="H64" s="1">
-        <v>7.7319999999999993</v>
+        <v>7.665</v>
       </c>
       <c r="I64" s="1">
-        <v>7.7</v>
+        <v>7.875</v>
       </c>
       <c r="J64" s="1">
-        <v>7.6819999999999995</v>
+        <v>7.835</v>
       </c>
       <c r="K64" s="1">
-        <v>7.7180000000000009</v>
+        <v>7.875</v>
       </c>
       <c r="L64" s="1">
-        <v>10</v>
+        <v>9.6649999999999991</v>
       </c>
       <c r="M64" s="1">
-        <v>10</v>
+        <v>9.6649999999999991</v>
       </c>
       <c r="N64" s="1">
-        <v>8.6</v>
+        <v>9.6649999999999991</v>
       </c>
       <c r="O64" s="1">
-        <v>7.831999999999999</v>
+        <v>8.2100000000000009</v>
       </c>
       <c r="P64" s="1">
-        <v>82.963999999999999</v>
+        <v>76.16</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="1">
-        <v>0.52633270930982268</v>
+        <v>11</v>
+      </c>
+      <c r="E65" s="4">
+        <v>1.2522872517992589</v>
       </c>
       <c r="F65" s="1">
-        <v>7.67</v>
+        <v>6.83</v>
       </c>
       <c r="G65" s="1">
-        <v>7.665</v>
+        <v>7.125</v>
       </c>
       <c r="H65" s="1">
-        <v>7.17</v>
+        <v>7.0449999999999999</v>
       </c>
       <c r="I65" s="1">
-        <v>7.33</v>
+        <v>6.835</v>
       </c>
       <c r="J65" s="1">
-        <v>7.875</v>
+        <v>7.375</v>
       </c>
       <c r="K65" s="1">
-        <v>7.25</v>
+        <v>7.08</v>
       </c>
       <c r="L65" s="1">
         <v>10</v>
@@ -3928,63 +3962,64 @@
         <v>10</v>
       </c>
       <c r="O65" s="1">
-        <v>7.5449999999999999</v>
+        <v>6.92</v>
       </c>
       <c r="P65" s="1">
-        <v>82.50500000000001</v>
+        <v>79.209999999999994</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E66" s="1">
-        <v>0.50523129525341992</v>
+      <c r="E66" s="4">
+        <v>0.69409714400530298</v>
       </c>
       <c r="F66" s="1">
-        <v>6.75</v>
+        <v>7.3866666666666667</v>
       </c>
       <c r="G66" s="1">
-        <v>6.67</v>
+        <v>7.2233333333333336</v>
       </c>
       <c r="H66" s="1">
-        <v>6.5</v>
+        <v>7.1400000000000006</v>
       </c>
       <c r="I66" s="1">
-        <v>6.83</v>
+        <v>7.1400000000000006</v>
       </c>
       <c r="J66" s="1">
-        <v>6.67</v>
+        <v>7.3900000000000006</v>
       </c>
       <c r="K66" s="1">
-        <v>6.92</v>
+        <v>7.4466666666666663</v>
       </c>
       <c r="L66" s="1">
-        <v>9.33</v>
+        <v>10</v>
       </c>
       <c r="M66" s="1">
-        <v>9.33</v>
+        <v>10</v>
       </c>
       <c r="N66" s="1">
-        <v>6.83</v>
+        <v>10</v>
       </c>
       <c r="O66" s="1">
-        <v>7.92</v>
+        <v>7.246666666666667</v>
       </c>
       <c r="P66" s="1">
-        <v>73.75</v>
+        <v>80.973333333333329</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P66" xr:uid="{51B2AF4A-2782-4D5A-A991-91E633920B43}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>